<commit_message>
add some gather event #86
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Drop.xlsx
+++ b/ConfigData/Xlsx/Drop.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17571"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -73,12 +73,30 @@
   <si>
     <t>水池</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>22010201;35|22010202;10|22010203;5|22010204;5</t>
+  </si>
+  <si>
+    <t>22010401;30|22010402;15|22010403;10</t>
+  </si>
+  <si>
+    <t>22010501;30|22010502;15|22010302;8</t>
+  </si>
+  <si>
+    <t>沙堆</t>
+  </si>
+  <si>
+    <t>蘑菇</t>
+  </si>
+  <si>
+    <t>枯木</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -953,74 +971,6 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1033,10 +983,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:D4" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" tableBorderDxfId="4">
-  <autoFilter ref="A3:D4"/>
-  <sortState ref="A4:O83">
-    <sortCondition ref="A3:A83"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:D7" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" tableBorderDxfId="4">
+  <autoFilter ref="A3:D7"/>
+  <sortState ref="A4:O82">
+    <sortCondition ref="A3:A82"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" name="Id" dataDxfId="3"/>
@@ -1049,14 +999,14 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CAEACD"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1124,6 +1074,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1159,6 +1126,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1335,13 +1319,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="B5" sqref="B5:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1407,6 +1391,48 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>23000002</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>23000003</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>23000004</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="3">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
finish the drop of equip
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Drop.xlsx
+++ b/ConfigData/Xlsx/Drop.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -91,6 +91,18 @@
   </si>
   <si>
     <t>枯木</t>
+  </si>
+  <si>
+    <t>装备等级</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>EquipLevel</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -983,15 +995,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:D7" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" tableBorderDxfId="4">
-  <autoFilter ref="A3:D7"/>
-  <sortState ref="A4:O82">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:E7" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" tableBorderDxfId="4">
+  <autoFilter ref="A3:E7"/>
+  <sortState ref="A4:P82">
     <sortCondition ref="A3:A82"/>
   </sortState>
-  <tableColumns count="4">
+  <tableColumns count="5">
     <tableColumn id="1" name="Id" dataDxfId="3"/>
     <tableColumn id="2" name="~Name" dataDxfId="2"/>
     <tableColumn id="12" name="Items" dataDxfId="1"/>
+    <tableColumn id="3" name="EquipLevel"/>
     <tableColumn id="13" name="Count" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1319,23 +1332,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5:B7"/>
+      <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.25" customWidth="1"/>
     <col min="3" max="3" width="78.375" customWidth="1"/>
-    <col min="4" max="4" width="9.5" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
+    <col min="5" max="5" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -1345,11 +1359,14 @@
       <c r="C1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1360,10 +1377,13 @@
         <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1374,10 +1394,13 @@
         <v>6</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>23000001</v>
       </c>
@@ -1387,11 +1410,12 @@
       <c r="C4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="3"/>
+      <c r="E4" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>23000002</v>
       </c>
@@ -1401,11 +1425,11 @@
       <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="3">
+      <c r="E5" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>23000003</v>
       </c>
@@ -1415,11 +1439,11 @@
       <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="3">
+      <c r="E6" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>23000004</v>
       </c>
@@ -1429,7 +1453,7 @@
       <c r="C7" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="3">
+      <c r="E7" s="3">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add the bat event
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Drop.xlsx
+++ b/ConfigData/Xlsx/Drop.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17766"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -149,14 +149,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>22010501;30|22010502;15|22010503;4|22010504;3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>22010401;30|22010402;15|22010403;7</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>素材袋</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -316,12 +308,20 @@
   </si>
   <si>
     <t>资源袋(石像)</t>
+  </si>
+  <si>
+    <t>22010301;30|22010302;15|22010303;7</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>22010401;30|22010402;15|22010403;4|22010404;3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1217,74 +1217,6 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1315,14 +1247,14 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CAEACD"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1390,6 +1322,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1425,6 +1374,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1604,10 +1570,10 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B18" sqref="B18:B40"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1734,7 +1700,7 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>85</v>
       </c>
       <c r="F7" s="3">
         <v>3</v>
@@ -1748,7 +1714,7 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>86</v>
       </c>
       <c r="F8" s="3">
         <v>3</v>
@@ -1829,7 +1795,7 @@
         <v>23000201</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E14" t="s">
         <v>26</v>
@@ -1843,7 +1809,7 @@
         <v>23000202</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E15" t="s">
         <v>27</v>
@@ -1857,7 +1823,7 @@
         <v>23000203</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E16" t="s">
         <v>28</v>
@@ -1871,7 +1837,7 @@
         <v>23000204</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E17" t="s">
         <v>29</v>
@@ -1885,10 +1851,10 @@
         <v>23000301</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F18" s="3">
         <v>3</v>
@@ -1899,10 +1865,10 @@
         <v>23000302</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F19" s="3">
         <v>3</v>
@@ -1913,10 +1879,10 @@
         <v>23000303</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F20" s="3">
         <v>3</v>
@@ -1927,10 +1893,10 @@
         <v>23000304</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F21" s="3">
         <v>3</v>
@@ -1941,10 +1907,10 @@
         <v>23000305</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F22" s="3">
         <v>3</v>
@@ -1955,10 +1921,10 @@
         <v>23000306</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F23" s="3">
         <v>3</v>
@@ -1969,10 +1935,10 @@
         <v>23000307</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F24" s="3">
         <v>3</v>
@@ -1983,10 +1949,10 @@
         <v>23000401</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F25" s="3">
         <v>3</v>
@@ -1997,10 +1963,10 @@
         <v>23000402</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F26" s="3">
         <v>3</v>
@@ -2011,10 +1977,10 @@
         <v>23000403</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F27" s="3">
         <v>3</v>
@@ -2025,10 +1991,10 @@
         <v>23000404</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F28" s="3">
         <v>3</v>
@@ -2039,10 +2005,10 @@
         <v>23000405</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F29" s="3">
         <v>3</v>
@@ -2053,10 +2019,10 @@
         <v>23000406</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F30" s="3">
         <v>3</v>
@@ -2067,10 +2033,10 @@
         <v>23000407</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F31" s="3">
         <v>3</v>
@@ -2081,10 +2047,10 @@
         <v>23000408</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F32" s="3">
         <v>3</v>
@@ -2095,10 +2061,10 @@
         <v>23000409</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F33" s="3">
         <v>3</v>
@@ -2109,10 +2075,10 @@
         <v>23000410</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F34" s="3">
         <v>3</v>
@@ -2123,10 +2089,10 @@
         <v>23000411</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F35" s="3">
         <v>3</v>
@@ -2137,10 +2103,10 @@
         <v>23000412</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F36" s="3">
         <v>3</v>
@@ -2151,10 +2117,10 @@
         <v>23000413</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F37" s="3">
         <v>3</v>
@@ -2165,10 +2131,10 @@
         <v>23000414</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F38" s="3">
         <v>3</v>
@@ -2179,10 +2145,10 @@
         <v>23000415</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F39" s="3">
         <v>3</v>
@@ -2193,10 +2159,10 @@
         <v>23000416</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F40" s="3">
         <v>3</v>

</xml_diff>

<commit_message>
rearrange the equip attrs. no equip level now
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Drop.xlsx
+++ b/ConfigData/Xlsx/Drop.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18067"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -78,18 +78,10 @@
     <t>枯木</t>
   </si>
   <si>
-    <t>装备等级</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>EquipLevel</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>随机Lv1装备</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -315,6 +307,26 @@
   </si>
   <si>
     <t>22010401;30|22010402;15|22010403;4|22010404;3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>装备品质最低</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>装备品质最高</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>EquipQualityMin</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>EquipQualityMax</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1229,16 +1241,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:F40" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" tableBorderDxfId="4">
-  <autoFilter ref="A3:F40"/>
-  <sortState ref="A4:P82">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:G40" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" tableBorderDxfId="4">
+  <autoFilter ref="A3:G40"/>
+  <sortState ref="A4:Q82">
     <sortCondition ref="A3:A82"/>
   </sortState>
-  <tableColumns count="6">
+  <tableColumns count="7">
     <tableColumn id="1" name="Id" dataDxfId="3"/>
     <tableColumn id="2" name="~Name" dataDxfId="2"/>
     <tableColumn id="12" name="Items" dataDxfId="1"/>
-    <tableColumn id="3" name="EquipLevel"/>
+    <tableColumn id="3" name="EquipQualityMin"/>
+    <tableColumn id="5" name="EquipQualityMax"/>
     <tableColumn id="4" name="RandomItemRate"/>
     <tableColumn id="13" name="Count" dataDxfId="0"/>
   </tableColumns>
@@ -1567,13 +1580,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1581,12 +1594,12 @@
     <col min="1" max="1" width="9.25" customWidth="1"/>
     <col min="2" max="2" width="13.375" customWidth="1"/>
     <col min="3" max="3" width="65.875" customWidth="1"/>
-    <col min="4" max="4" width="4.25" customWidth="1"/>
-    <col min="5" max="5" width="15.875" customWidth="1"/>
-    <col min="6" max="6" width="4.25" customWidth="1"/>
+    <col min="4" max="5" width="4.25" customWidth="1"/>
+    <col min="6" max="6" width="15.875" customWidth="1"/>
+    <col min="7" max="7" width="4.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -1597,16 +1610,19 @@
         <v>7</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>15</v>
+        <v>85</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1617,16 +1633,19 @@
         <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>30</v>
+        <v>87</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1637,32 +1656,36 @@
         <v>6</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>17</v>
+        <v>88</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>25</v>
+        <v>89</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>23000001</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="F4" s="3"/>
+      <c r="G4" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>23000002</v>
       </c>
@@ -1670,29 +1693,30 @@
         <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+        <v>30</v>
+      </c>
+      <c r="G5" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>23000003</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
-      <c r="F6" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="F6" s="3"/>
+      <c r="G6" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>23000004</v>
       </c>
@@ -1700,13 +1724,13 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>85</v>
-      </c>
-      <c r="F7" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+        <v>83</v>
+      </c>
+      <c r="G7" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>23000005</v>
       </c>
@@ -1714,465 +1738,480 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>86</v>
-      </c>
-      <c r="F8" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+        <v>84</v>
+      </c>
+      <c r="G8" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>23000101</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="G9" s="3">
         <v>1</v>
       </c>
-      <c r="F9" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>23000102</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D10">
-        <v>2</v>
-      </c>
-      <c r="F10" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>23000103</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D11">
-        <v>3</v>
-      </c>
-      <c r="F11" s="3">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="G11" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>23000104</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D12">
-        <v>4</v>
-      </c>
-      <c r="F12" s="3">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="G12" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>23000105</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D13">
-        <v>5</v>
-      </c>
-      <c r="F13" s="3">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="G13" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>23000201</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E14" t="s">
-        <v>26</v>
-      </c>
-      <c r="F14" s="3">
+        <v>33</v>
+      </c>
+      <c r="F14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>23000202</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="3">
+        <v>34</v>
+      </c>
+      <c r="F15" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>23000203</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F16" s="3">
+        <v>35</v>
+      </c>
+      <c r="F16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>23000204</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E17" t="s">
-        <v>29</v>
-      </c>
-      <c r="F17" s="3">
+        <v>36</v>
+      </c>
+      <c r="F17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>23000301</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F18" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+        <v>37</v>
+      </c>
+      <c r="G18" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>23000302</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
-      </c>
-      <c r="F19" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+        <v>38</v>
+      </c>
+      <c r="G19" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>23000303</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C20" t="s">
-        <v>41</v>
-      </c>
-      <c r="F20" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+        <v>39</v>
+      </c>
+      <c r="G20" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>23000304</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
-      </c>
-      <c r="F21" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+        <v>40</v>
+      </c>
+      <c r="G21" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>23000305</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
-      </c>
-      <c r="F22" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+        <v>41</v>
+      </c>
+      <c r="G22" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>23000306</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C23" t="s">
-        <v>44</v>
-      </c>
-      <c r="F23" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+        <v>42</v>
+      </c>
+      <c r="G23" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>23000307</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="F24" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+        <v>43</v>
+      </c>
+      <c r="G24" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>23000401</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F25" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+        <v>44</v>
+      </c>
+      <c r="G25" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>23000402</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="F26" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
+        <v>45</v>
+      </c>
+      <c r="G26" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>23000403</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="F27" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
+        <v>46</v>
+      </c>
+      <c r="G27" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>23000404</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="F28" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
+        <v>47</v>
+      </c>
+      <c r="G28" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>23000405</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F29" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
+        <v>48</v>
+      </c>
+      <c r="G29" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>23000406</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="F30" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
+        <v>49</v>
+      </c>
+      <c r="G30" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>23000407</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="F31" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
+        <v>50</v>
+      </c>
+      <c r="G31" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>23000408</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="F32" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
+        <v>51</v>
+      </c>
+      <c r="G32" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>23000409</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="F33" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
+        <v>52</v>
+      </c>
+      <c r="G33" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>23000410</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="F34" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
+        <v>53</v>
+      </c>
+      <c r="G34" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>23000411</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="F35" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
+        <v>54</v>
+      </c>
+      <c r="G35" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>23000412</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="F36" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
+        <v>55</v>
+      </c>
+      <c r="G36" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>23000413</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="F37" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
+        <v>56</v>
+      </c>
+      <c r="G37" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>23000414</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="F38" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
+        <v>57</v>
+      </c>
+      <c r="G38" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>23000415</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="F39" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
+        <v>58</v>
+      </c>
+      <c r="G39" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>23000416</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="F40" s="3">
+        <v>59</v>
+      </c>
+      <c r="G40" s="3">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="E14:E17">
+  <conditionalFormatting sqref="F14:F17">
     <cfRule type="containsBlanks" dxfId="7" priority="1">
-      <formula>LEN(TRIM(E14))=0</formula>
+      <formula>LEN(TRIM(F14))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
use item ename as the key of item data
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Drop.xlsx
+++ b/ConfigData/Xlsx/Drop.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Drop" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="98">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -64,10 +64,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>RLIdValueList</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>水池</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -128,15 +124,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>22010001;32|22010002;28|22010003;15|22010004;12|22010005;6|22010006;4|22010007;2|22010008;1</t>
-  </si>
-  <si>
-    <t>22010101;32|22010102;28|22010103;15|22010104;12|22010105;6|22010106;4|22010107;2|22010108;1</t>
-  </si>
-  <si>
-    <t>22010201;32|22010202;28|22010203;15|22010204;12|22010205;6|22010206;4|22010207;2|22010208;1</t>
-  </si>
-  <si>
     <t>草丛</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -157,75 +144,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>22018001;52|22018002;28|22018003;15|22018004;5</t>
-  </si>
-  <si>
-    <t>22018011;52|22018012;28|22018013;15|22018014;5</t>
-  </si>
-  <si>
-    <t>22018021;52|22018022;28|22018023;15|22018024;5</t>
-  </si>
-  <si>
-    <t>22018031;52|22018032;28|22018033;15|22018034;5</t>
-  </si>
-  <si>
-    <t>22018041;52|22018042;28|22018043;15|22018044;5</t>
-  </si>
-  <si>
-    <t>22018051;52|22018052;28|22018053;15|22018054;5</t>
-  </si>
-  <si>
-    <t>22018061;52|22018062;28|22018063;15|22018064;5</t>
-  </si>
-  <si>
-    <t>22019011;64|22019012;23|22019013;10|22019014;3</t>
-  </si>
-  <si>
-    <t>22019021;64|22019022;23|22019023;10|22019024;3</t>
-  </si>
-  <si>
-    <t>22019031;64|22019032;23|22019033;10|22019034;3</t>
-  </si>
-  <si>
-    <t>22019041;64|22019042;23|22019043;10|22019044;3</t>
-  </si>
-  <si>
-    <t>22019051;64|22019052;23|22019053;10|22019054;3</t>
-  </si>
-  <si>
-    <t>22019061;64|22019062;23|22019063;10|22019064;3</t>
-  </si>
-  <si>
-    <t>22019071;64|22019072;23|22019073;10|22019074;3</t>
-  </si>
-  <si>
-    <t>22019081;64|22019082;23|22019083;10|22019084;3</t>
-  </si>
-  <si>
-    <t>22019091;64|22019092;23|22019093;10|22019094;3</t>
-  </si>
-  <si>
-    <t>22019101;64|22019102;23|22019103;10|22019104;3</t>
-  </si>
-  <si>
-    <t>22019111;64|22019112;23|22019113;10|22019114;3</t>
-  </si>
-  <si>
-    <t>22019121;64|22019122;23|22019123;10|22019124;3</t>
-  </si>
-  <si>
-    <t>22019131;64|22019132;23|22019133;10|22019134;3</t>
-  </si>
-  <si>
-    <t>22019141;64|22019142;23|22019143;10|22019144;3</t>
-  </si>
-  <si>
-    <t>22019151;64|22019152;23|22019153;10|22019154;3</t>
-  </si>
-  <si>
-    <t>22019161;64|22019162;23|22019163;10|22019164;3</t>
-  </si>
-  <si>
     <t>素材袋(无)</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -302,14 +220,6 @@
     <t>资源袋(石像)</t>
   </si>
   <si>
-    <t>22010301;30|22010302;15|22010303;7</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>22010401;30|22010402;15|22010403;4|22010404;3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>装备品质最低</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -327,6 +237,121 @@
   </si>
   <si>
     <t>EquipQualityMax</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>zycao1;zycao2;zycao3;zycao4;zycao5;zycao6;zycao7;zycao8</t>
+  </si>
+  <si>
+    <t>zyyu1;zyyu2;zyyu3;zyyu4;zyyu5;zyyu6;zyyu7;zyyu8</t>
+  </si>
+  <si>
+    <t>zyshi1;zyshi2;zyshi3;zyshi4;zyshi5;zyshi6;zyshi7;zyshi8</t>
+  </si>
+  <si>
+    <t>zygu1;zygu2;zygu3</t>
+  </si>
+  <si>
+    <t>zymu1;zymu2;zymu3;zymu4</t>
+  </si>
+  <si>
+    <t>scwu1;scwu2;scwu3;scwu4</t>
+  </si>
+  <si>
+    <t>scshui1;scshui2;scshui3;scshui4</t>
+  </si>
+  <si>
+    <t>scfeng1;scfeng2;scfeng3;scfeng4</t>
+  </si>
+  <si>
+    <t>schuo1;schuo2;schuo3;schuo4</t>
+  </si>
+  <si>
+    <t>scdi1;scdi2;scdi3;scdi4</t>
+  </si>
+  <si>
+    <t>scguang1;scguang2;scguang3;scguang4</t>
+  </si>
+  <si>
+    <t>scan1;scan2;scan3;scan4</t>
+  </si>
+  <si>
+    <t>scemo1;scemo2;scemo3;scemo4</t>
+  </si>
+  <si>
+    <t>scjixie1;scjixie2;scjixie3;scjixie4</t>
+  </si>
+  <si>
+    <t>scjingling1;scjingling2;scjingling3;scjingling4</t>
+  </si>
+  <si>
+    <t>sckunchong1;sckunchong2;sckunchong3;sckunchong4</t>
+  </si>
+  <si>
+    <t>sclong1;sclong2;sclong3;sclong4</t>
+  </si>
+  <si>
+    <t>scniao1;scniao2;scniao3;scniao4</t>
+  </si>
+  <si>
+    <t>scpaxing1;scpaxing2;scpaxing3;scpaxing4</t>
+  </si>
+  <si>
+    <t>screnlei1;screnlei2;screnlei3;screnlei4</t>
+  </si>
+  <si>
+    <t>scshouren1;scshouren2;scshouren3;scshouren4</t>
+  </si>
+  <si>
+    <t>scwangling1;scwangling2;scwangling3;scwangling4</t>
+  </si>
+  <si>
+    <t>scyeshou1;scyeshou2;scyeshou3;scyeshou4</t>
+  </si>
+  <si>
+    <t>scyu1;scyu2;scyu3;scyu4</t>
+  </si>
+  <si>
+    <t>scyuansu1;scyuansu2;scyuansu3;scyuansu4</t>
+  </si>
+  <si>
+    <t>sczhiwu1;sczhiwu2;sczhiwu3;sczhiwu4</t>
+  </si>
+  <si>
+    <t>scdijing1;scdijing2;scdijing3;scdijing4</t>
+  </si>
+  <si>
+    <t>sctuteng1;sctuteng2;sctuteng3;sctuteng4</t>
+  </si>
+  <si>
+    <t>32;28;15;12;6;4;2;1</t>
+  </si>
+  <si>
+    <t>30;15;7</t>
+  </si>
+  <si>
+    <t>30;15;4;3</t>
+  </si>
+  <si>
+    <t>52;28;15;5</t>
+  </si>
+  <si>
+    <t>64;23;10;3</t>
+  </si>
+  <si>
+    <t>string[]</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int[]</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ItemRate</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>掉落概率</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -979,7 +1004,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1005,6 +1030,12 @@
       <alignment vertical="center" textRotation="255" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1052,7 +1083,36 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1217,16 +1277,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1241,19 +1291,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:G40" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" tableBorderDxfId="4">
-  <autoFilter ref="A3:G40"/>
-  <sortState ref="A4:Q82">
-    <sortCondition ref="A3:A82"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:H40" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" tableBorderDxfId="6">
+  <autoFilter ref="A3:H40"/>
+  <sortState ref="A4:R81">
+    <sortCondition ref="A3:A81"/>
   </sortState>
-  <tableColumns count="7">
-    <tableColumn id="1" name="Id" dataDxfId="3"/>
-    <tableColumn id="2" name="~Name" dataDxfId="2"/>
-    <tableColumn id="12" name="Items" dataDxfId="1"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="Id" dataDxfId="5"/>
+    <tableColumn id="2" name="~Name" dataDxfId="4"/>
+    <tableColumn id="12" name="Items" dataDxfId="3"/>
+    <tableColumn id="6" name="ItemRate" dataDxfId="0"/>
     <tableColumn id="3" name="EquipQualityMin"/>
     <tableColumn id="5" name="EquipQualityMax"/>
     <tableColumn id="4" name="RandomItemRate"/>
-    <tableColumn id="13" name="Count" dataDxfId="0"/>
+    <tableColumn id="13" name="Count" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1580,26 +1631,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.25" customWidth="1"/>
     <col min="2" max="2" width="13.375" customWidth="1"/>
-    <col min="3" max="3" width="65.875" customWidth="1"/>
-    <col min="4" max="5" width="4.25" customWidth="1"/>
-    <col min="6" max="6" width="15.875" customWidth="1"/>
-    <col min="7" max="7" width="4.25" customWidth="1"/>
+    <col min="3" max="3" width="48.75" customWidth="1"/>
+    <col min="4" max="4" width="21.875" customWidth="1"/>
+    <col min="5" max="6" width="4.25" customWidth="1"/>
+    <col min="7" max="7" width="15.875" customWidth="1"/>
+    <col min="8" max="8" width="4.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -1610,19 +1662,22 @@
         <v>7</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>86</v>
+        <v>56</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1630,22 +1685,25 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>94</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>95</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>87</v>
+        <v>14</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1656,562 +1714,649 @@
         <v>6</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>89</v>
+        <v>59</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="G3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>23000001</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="3"/>
+        <v>61</v>
+      </c>
+      <c r="D4" t="s">
+        <v>89</v>
+      </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G4" s="3"/>
+      <c r="H4" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>23000002</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+        <v>62</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="H5" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>23000003</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="3"/>
+        <v>63</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G6" s="3"/>
+      <c r="H6" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>23000004</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>83</v>
-      </c>
-      <c r="G7" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+        <v>64</v>
+      </c>
+      <c r="D7" t="s">
+        <v>90</v>
+      </c>
+      <c r="H7" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>23000005</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>84</v>
-      </c>
-      <c r="G8" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+        <v>65</v>
+      </c>
+      <c r="D8" t="s">
+        <v>91</v>
+      </c>
+      <c r="H8" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>23000101</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9">
+        <v>15</v>
+      </c>
+      <c r="E9">
         <v>0</v>
       </c>
-      <c r="E9">
-        <v>3</v>
-      </c>
-      <c r="G9" s="3">
+      <c r="F9">
+        <v>3</v>
+      </c>
+      <c r="H9" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>23000102</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10">
+        <v>16</v>
+      </c>
+      <c r="E10">
         <v>1</v>
       </c>
-      <c r="E10">
-        <v>3</v>
-      </c>
-      <c r="G10" s="3">
+      <c r="F10">
+        <v>3</v>
+      </c>
+      <c r="H10" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>23000103</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11">
+        <v>17</v>
+      </c>
+      <c r="E11">
         <v>2</v>
       </c>
-      <c r="E11">
-        <v>3</v>
-      </c>
-      <c r="G11" s="3">
+      <c r="F11">
+        <v>3</v>
+      </c>
+      <c r="H11" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>23000104</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="E12">
         <v>3</v>
       </c>
-      <c r="G12" s="3">
+      <c r="F12">
+        <v>3</v>
+      </c>
+      <c r="H12" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>23000105</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="E13">
         <v>4</v>
       </c>
-      <c r="G13" s="3">
+      <c r="F13">
+        <v>4</v>
+      </c>
+      <c r="H13" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>23000201</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" t="s">
-        <v>24</v>
-      </c>
-      <c r="G14" s="3">
+        <v>29</v>
+      </c>
+      <c r="G14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>23000202</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F15" t="s">
-        <v>25</v>
-      </c>
-      <c r="G15" s="3">
+        <v>30</v>
+      </c>
+      <c r="G15" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>23000203</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F16" t="s">
-        <v>26</v>
-      </c>
-      <c r="G16" s="3">
+        <v>31</v>
+      </c>
+      <c r="G16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>23000204</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F17" t="s">
-        <v>27</v>
-      </c>
-      <c r="G17" s="3">
+        <v>32</v>
+      </c>
+      <c r="G17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>23000301</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
-      </c>
-      <c r="G18" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+        <v>66</v>
+      </c>
+      <c r="D18" t="s">
+        <v>92</v>
+      </c>
+      <c r="H18" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>23000302</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
-      </c>
-      <c r="G19" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
+        <v>67</v>
+      </c>
+      <c r="D19" t="s">
+        <v>92</v>
+      </c>
+      <c r="H19" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>23000303</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
-      </c>
-      <c r="G20" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
+        <v>68</v>
+      </c>
+      <c r="D20" t="s">
+        <v>92</v>
+      </c>
+      <c r="H20" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>23000304</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
-      </c>
-      <c r="G21" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
+        <v>69</v>
+      </c>
+      <c r="D21" t="s">
+        <v>92</v>
+      </c>
+      <c r="H21" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>23000305</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="C22" t="s">
-        <v>41</v>
-      </c>
-      <c r="G22" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
+        <v>70</v>
+      </c>
+      <c r="D22" t="s">
+        <v>92</v>
+      </c>
+      <c r="H22" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>23000306</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>65</v>
+        <v>38</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
-      </c>
-      <c r="G23" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
+        <v>71</v>
+      </c>
+      <c r="D23" t="s">
+        <v>92</v>
+      </c>
+      <c r="H23" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>23000307</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G24" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
+        <v>72</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="H24" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>23000401</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="G25" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
+        <v>73</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="H25" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>23000402</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="G26" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
+        <v>74</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="H26" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>23000403</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="G27" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
+        <v>75</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="H27" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>23000404</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="G28" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
+        <v>76</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="H28" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>23000405</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>71</v>
+        <v>44</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="G29" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
+        <v>77</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="H29" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>23000406</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="G30" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
+        <v>78</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="H30" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>23000407</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>73</v>
+        <v>46</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="G31" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
+        <v>79</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="H31" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>23000408</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="G32" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
+        <v>80</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="H32" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>23000409</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>75</v>
+        <v>48</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G33" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="H33" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>23000410</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>76</v>
+        <v>49</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="G34" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
+        <v>82</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="H34" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>23000411</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="G35" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
+        <v>83</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="H35" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>23000412</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="G36" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
+        <v>84</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="H36" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>23000413</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="G37" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
+        <v>85</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="H37" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>23000414</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>80</v>
+        <v>53</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="G38" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
+        <v>86</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="H38" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>23000415</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="G39" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
+        <v>87</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="H39" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>23000416</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="G40" s="3">
+        <v>88</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="H40" s="3">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="F14:F17">
-    <cfRule type="containsBlanks" dxfId="7" priority="1">
-      <formula>LEN(TRIM(F14))=0</formula>
+  <conditionalFormatting sqref="G14:G17">
+    <cfRule type="containsBlanks" dxfId="1" priority="1">
+      <formula>LEN(TRIM(G14))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add drop name column
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Drop.xlsx
+++ b/ConfigData/Xlsx/Drop.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="137">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -352,6 +352,136 @@
   </si>
   <si>
     <t>掉落概率</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ename</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>英文名</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dlsuijilv3zhuangbei</t>
+  </si>
+  <si>
+    <t>dlsuijilv4zhuangbei</t>
+  </si>
+  <si>
+    <t>dlsuijilv5zhuangbei</t>
+  </si>
+  <si>
+    <t>dlsucaidai(wu)</t>
+  </si>
+  <si>
+    <t>dlsucaidai(shui)</t>
+  </si>
+  <si>
+    <t>dlsucaidai(feng)</t>
+  </si>
+  <si>
+    <t>dlsucaidai(huo)</t>
+  </si>
+  <si>
+    <t>dlsucaidai(di)</t>
+  </si>
+  <si>
+    <t>dlsucaidai(guang)</t>
+  </si>
+  <si>
+    <t>dlsucaidai(an)</t>
+  </si>
+  <si>
+    <t>dlziyuandai(emo)</t>
+  </si>
+  <si>
+    <t>dlziyuandai(jixie)</t>
+  </si>
+  <si>
+    <t>dlziyuandai(jingling)</t>
+  </si>
+  <si>
+    <t>dlziyuandai(kunchong)</t>
+  </si>
+  <si>
+    <t>dlziyuandai(long)</t>
+  </si>
+  <si>
+    <t>dlziyuandai(niao)</t>
+  </si>
+  <si>
+    <t>dlziyuandai(paxing)</t>
+  </si>
+  <si>
+    <t>dlziyuandai(renlei)</t>
+  </si>
+  <si>
+    <t>dlziyuandai(shouren)</t>
+  </si>
+  <si>
+    <t>dlziyuandai(wangling)</t>
+  </si>
+  <si>
+    <t>dlziyuandai(yeshou)</t>
+  </si>
+  <si>
+    <t>dlziyuandai(yu)</t>
+  </si>
+  <si>
+    <t>dlziyuandai(yuansu)</t>
+  </si>
+  <si>
+    <t>dlziyuandai(zhiwu)</t>
+  </si>
+  <si>
+    <t>dlziyuandai(dijing)</t>
+  </si>
+  <si>
+    <t>dlziyuandai(shixiang)</t>
+  </si>
+  <si>
+    <t>dlcao</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dlyu</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dlshi</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dlgu</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dlmu</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dlsucaidai</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dlsucaidaigaoji</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dlsucaidaiteji</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dlsucaidaijipin</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dlsuijilv2zhuangbei</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dlsuijilv1zhuangbei</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1083,7 +1213,17 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1098,20 +1238,20 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
-        <family val="3"/>
+        <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1139,6 +1279,25 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1291,16 +1450,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:H40" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" tableBorderDxfId="6">
-  <autoFilter ref="A3:H40"/>
-  <sortState ref="A4:R81">
-    <sortCondition ref="A3:A81"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:I40" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7">
+  <autoFilter ref="A3:I40"/>
+  <sortState ref="A4:S80">
+    <sortCondition ref="A3:A80"/>
   </sortState>
-  <tableColumns count="8">
-    <tableColumn id="1" name="Id" dataDxfId="5"/>
-    <tableColumn id="2" name="~Name" dataDxfId="4"/>
-    <tableColumn id="12" name="Items" dataDxfId="3"/>
-    <tableColumn id="6" name="ItemRate" dataDxfId="0"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="Id" dataDxfId="6"/>
+    <tableColumn id="2" name="~Name" dataDxfId="5"/>
+    <tableColumn id="7" name="Ename" dataDxfId="1"/>
+    <tableColumn id="12" name="Items" dataDxfId="4"/>
+    <tableColumn id="6" name="ItemRate" dataDxfId="3"/>
     <tableColumn id="3" name="EquipQualityMin"/>
     <tableColumn id="5" name="EquipQualityMax"/>
     <tableColumn id="4" name="RandomItemRate"/>
@@ -1631,27 +1791,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.25" customWidth="1"/>
     <col min="2" max="2" width="13.375" customWidth="1"/>
-    <col min="3" max="3" width="48.75" customWidth="1"/>
-    <col min="4" max="4" width="21.875" customWidth="1"/>
-    <col min="5" max="6" width="4.25" customWidth="1"/>
-    <col min="7" max="7" width="15.875" customWidth="1"/>
-    <col min="8" max="8" width="4.25" customWidth="1"/>
+    <col min="3" max="3" width="9.875" customWidth="1"/>
+    <col min="4" max="4" width="48.75" customWidth="1"/>
+    <col min="5" max="5" width="21.875" customWidth="1"/>
+    <col min="6" max="7" width="4.25" customWidth="1"/>
+    <col min="8" max="8" width="15.875" customWidth="1"/>
+    <col min="9" max="9" width="4.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -1659,25 +1820,28 @@
         <v>3</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1685,25 +1849,28 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1711,45 +1878,51 @@
         <v>5</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>23000001</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="D4" t="s">
         <v>61</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>89</v>
       </c>
-      <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="H4" s="3"/>
+      <c r="I4" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>23000002</v>
       </c>
@@ -1757,36 +1930,42 @@
         <v>11</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="E5" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="H5" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I5" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>23000003</v>
       </c>
       <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="H6" s="3"/>
+      <c r="I6" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>23000004</v>
       </c>
@@ -1794,16 +1973,19 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
+        <v>129</v>
+      </c>
+      <c r="D7" t="s">
         <v>64</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>90</v>
       </c>
-      <c r="H7" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I7" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>23000005</v>
       </c>
@@ -1811,259 +1993,307 @@
         <v>13</v>
       </c>
       <c r="C8" t="s">
+        <v>130</v>
+      </c>
+      <c r="D8" t="s">
         <v>65</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>91</v>
       </c>
-      <c r="H8" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I8" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>23000101</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
       </c>
-      <c r="E9">
+      <c r="C9" t="s">
+        <v>136</v>
+      </c>
+      <c r="F9">
         <v>0</v>
       </c>
-      <c r="F9">
-        <v>3</v>
-      </c>
-      <c r="H9" s="3">
+      <c r="G9">
+        <v>3</v>
+      </c>
+      <c r="I9" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>23000102</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
       </c>
-      <c r="E10">
+      <c r="C10" t="s">
+        <v>135</v>
+      </c>
+      <c r="F10">
         <v>1</v>
       </c>
-      <c r="F10">
-        <v>3</v>
-      </c>
-      <c r="H10" s="3">
+      <c r="G10">
+        <v>3</v>
+      </c>
+      <c r="I10" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>23000103</v>
       </c>
       <c r="B11" t="s">
         <v>17</v>
       </c>
-      <c r="E11">
+      <c r="C11" t="s">
+        <v>100</v>
+      </c>
+      <c r="F11">
         <v>2</v>
       </c>
-      <c r="F11">
-        <v>3</v>
-      </c>
-      <c r="H11" s="3">
+      <c r="G11">
+        <v>3</v>
+      </c>
+      <c r="I11" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>23000104</v>
       </c>
       <c r="B12" t="s">
         <v>18</v>
       </c>
-      <c r="E12">
-        <v>3</v>
+      <c r="C12" t="s">
+        <v>101</v>
       </c>
       <c r="F12">
         <v>3</v>
       </c>
-      <c r="H12" s="3">
+      <c r="G12">
+        <v>3</v>
+      </c>
+      <c r="I12" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>23000105</v>
       </c>
       <c r="B13" t="s">
         <v>19</v>
       </c>
-      <c r="E13">
-        <v>4</v>
+      <c r="C13" t="s">
+        <v>102</v>
       </c>
       <c r="F13">
         <v>4</v>
       </c>
-      <c r="H13" s="3">
+      <c r="G13">
+        <v>4</v>
+      </c>
+      <c r="I13" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>23000201</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G14" t="s">
+      <c r="C14" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="H14" t="s">
         <v>23</v>
       </c>
-      <c r="H14" s="3">
+      <c r="I14" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>23000202</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G15" t="s">
+      <c r="C15" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="H15" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="3">
+      <c r="I15" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>23000203</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G16" t="s">
+      <c r="C16" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="H16" t="s">
         <v>25</v>
       </c>
-      <c r="H16" s="3">
+      <c r="I16" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>23000204</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G17" t="s">
+      <c r="C17" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="H17" t="s">
         <v>26</v>
       </c>
-      <c r="H17" s="3">
+      <c r="I17" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>23000301</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="D18" t="s">
         <v>66</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>92</v>
       </c>
-      <c r="H18" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I18" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>23000302</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="D19" t="s">
         <v>67</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>92</v>
       </c>
-      <c r="H19" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I19" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>23000303</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D20" t="s">
         <v>68</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>92</v>
       </c>
-      <c r="H20" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I20" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>23000304</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="D21" t="s">
         <v>69</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>92</v>
       </c>
-      <c r="H21" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I21" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>23000305</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="D22" t="s">
         <v>70</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>92</v>
       </c>
-      <c r="H22" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I22" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>23000306</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D23" t="s">
         <v>71</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>92</v>
       </c>
-      <c r="H23" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I23" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>23000307</v>
       </c>
@@ -2071,292 +2301,343 @@
         <v>39</v>
       </c>
       <c r="C24" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D24" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="E24" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="H24" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I24" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>23000401</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D25" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="E25" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H25" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I25" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>23000402</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D26" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="E26" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H26" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I26" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>23000403</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D27" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="E27" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H27" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I27" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>23000404</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D28" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="E28" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H28" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I28" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>23000405</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D29" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="E29" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H29" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I29" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>23000406</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D30" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="E30" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H30" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I30" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>23000407</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C31" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D31" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="E31" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H31" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I31" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>23000408</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D32" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="E32" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H32" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I32" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>23000409</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C33" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D33" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="E33" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H33" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I33" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>23000410</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D34" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="E34" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H34" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I34" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>23000411</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D35" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="D35" s="10" t="s">
+      <c r="E35" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H35" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I35" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>23000412</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D36" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="D36" s="10" t="s">
+      <c r="E36" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H36" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I36" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>23000413</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D37" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="D37" s="10" t="s">
+      <c r="E37" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H37" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I37" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>23000414</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="C38" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D38" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="D38" s="10" t="s">
+      <c r="E38" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H38" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I38" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>23000415</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D39" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D39" s="10" t="s">
+      <c r="E39" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H39" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I39" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>23000416</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="C40" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D40" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="D40" s="10" t="s">
+      <c r="E40" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H40" s="3">
+      <c r="I40" s="3">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="G14:G17">
-    <cfRule type="containsBlanks" dxfId="1" priority="1">
-      <formula>LEN(TRIM(G14))=0</formula>
+  <conditionalFormatting sqref="H14:H17">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(H14))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
trade support drop. add 2 scenequests
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Drop.xlsx
+++ b/ConfigData/Xlsx/Drop.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -40,10 +40,6 @@
     <t>Id</t>
   </si>
   <si>
-    <t>~Name</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>Items</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -482,6 +478,10 @@
   </si>
   <si>
     <t>dlsuijilv1zhuangbei</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1216,45 +1216,6 @@
   <dxfs count="10">
     <dxf>
       <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1313,6 +1274,35 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -1436,6 +1426,16 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1450,21 +1450,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:I40" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:I40" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" tableBorderDxfId="6">
   <autoFilter ref="A3:I40"/>
   <sortState ref="A4:S80">
     <sortCondition ref="A3:A80"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" name="Id" dataDxfId="6"/>
-    <tableColumn id="2" name="~Name" dataDxfId="5"/>
-    <tableColumn id="7" name="Ename" dataDxfId="1"/>
-    <tableColumn id="12" name="Items" dataDxfId="4"/>
-    <tableColumn id="6" name="ItemRate" dataDxfId="3"/>
+    <tableColumn id="1" name="Id" dataDxfId="5"/>
+    <tableColumn id="2" name="Name" dataDxfId="4"/>
+    <tableColumn id="7" name="Ename" dataDxfId="3"/>
+    <tableColumn id="12" name="Items" dataDxfId="2"/>
+    <tableColumn id="6" name="ItemRate" dataDxfId="1"/>
     <tableColumn id="3" name="EquipQualityMin"/>
     <tableColumn id="5" name="EquipQualityMax"/>
     <tableColumn id="4" name="RandomItemRate"/>
-    <tableColumn id="13" name="Count" dataDxfId="2"/>
+    <tableColumn id="13" name="Count" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1797,7 +1797,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1820,25 +1820,25 @@
         <v>3</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>7</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
@@ -1852,22 +1852,22 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>95</v>
-      </c>
       <c r="F2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
@@ -1875,28 +1875,28 @@
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>6</v>
-      </c>
       <c r="E3" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>60</v>
-      </c>
       <c r="H3" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
@@ -1904,16 +1904,16 @@
         <v>23000001</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -1927,16 +1927,16 @@
         <v>23000002</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I5" s="3">
         <v>3</v>
@@ -1947,16 +1947,16 @@
         <v>23000003</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -1970,16 +1970,16 @@
         <v>23000004</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I7" s="3">
         <v>3</v>
@@ -1990,16 +1990,16 @@
         <v>23000005</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I8" s="3">
         <v>3</v>
@@ -2010,10 +2010,10 @@
         <v>23000101</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -2030,10 +2030,10 @@
         <v>23000102</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -2050,10 +2050,10 @@
         <v>23000103</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F11">
         <v>2</v>
@@ -2070,10 +2070,10 @@
         <v>23000104</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F12">
         <v>3</v>
@@ -2090,10 +2090,10 @@
         <v>23000105</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F13">
         <v>4</v>
@@ -2110,13 +2110,13 @@
         <v>23000201</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I14" s="3">
         <v>2</v>
@@ -2127,13 +2127,13 @@
         <v>23000202</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I15" s="3">
         <v>4</v>
@@ -2144,13 +2144,13 @@
         <v>23000203</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I16" s="3">
         <v>6</v>
@@ -2161,13 +2161,13 @@
         <v>23000204</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I17" s="3">
         <v>8</v>
@@ -2178,16 +2178,16 @@
         <v>23000301</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I18" s="3">
         <v>3</v>
@@ -2198,16 +2198,16 @@
         <v>23000302</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I19" s="3">
         <v>3</v>
@@ -2218,16 +2218,16 @@
         <v>23000303</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I20" s="3">
         <v>3</v>
@@ -2238,16 +2238,16 @@
         <v>23000304</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I21" s="3">
         <v>3</v>
@@ -2258,16 +2258,16 @@
         <v>23000305</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I22" s="3">
         <v>3</v>
@@ -2278,16 +2278,16 @@
         <v>23000306</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I23" s="3">
         <v>3</v>
@@ -2298,16 +2298,16 @@
         <v>23000307</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I24" s="3">
         <v>3</v>
@@ -2318,16 +2318,16 @@
         <v>23000401</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I25" s="3">
         <v>3</v>
@@ -2338,16 +2338,16 @@
         <v>23000402</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I26" s="3">
         <v>3</v>
@@ -2358,16 +2358,16 @@
         <v>23000403</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I27" s="3">
         <v>3</v>
@@ -2378,16 +2378,16 @@
         <v>23000404</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I28" s="3">
         <v>3</v>
@@ -2398,16 +2398,16 @@
         <v>23000405</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I29" s="3">
         <v>3</v>
@@ -2418,16 +2418,16 @@
         <v>23000406</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I30" s="3">
         <v>3</v>
@@ -2438,16 +2438,16 @@
         <v>23000407</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I31" s="3">
         <v>3</v>
@@ -2458,16 +2458,16 @@
         <v>23000408</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I32" s="3">
         <v>3</v>
@@ -2478,16 +2478,16 @@
         <v>23000409</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I33" s="3">
         <v>3</v>
@@ -2498,16 +2498,16 @@
         <v>23000410</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I34" s="3">
         <v>3</v>
@@ -2518,16 +2518,16 @@
         <v>23000411</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I35" s="3">
         <v>3</v>
@@ -2538,16 +2538,16 @@
         <v>23000412</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I36" s="3">
         <v>3</v>
@@ -2558,16 +2558,16 @@
         <v>23000413</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I37" s="3">
         <v>3</v>
@@ -2578,16 +2578,16 @@
         <v>23000414</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I38" s="3">
         <v>3</v>
@@ -2598,16 +2598,16 @@
         <v>23000415</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I39" s="3">
         <v>3</v>
@@ -2618,16 +2618,16 @@
         <v>23000416</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I40" s="3">
         <v>3</v>
@@ -2636,7 +2636,7 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="H14:H17">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="9" priority="1">
       <formula>LEN(TRIM(H14))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add a new scene quest
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Drop.xlsx
+++ b/ConfigData/Xlsx/Drop.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="141">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -359,15 +359,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>dlsuijilv3zhuangbei</t>
-  </si>
-  <si>
-    <t>dlsuijilv4zhuangbei</t>
-  </si>
-  <si>
-    <t>dlsuijilv5zhuangbei</t>
-  </si>
-  <si>
     <t>dlsucaidai(wu)</t>
   </si>
   <si>
@@ -473,15 +464,39 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>dlsuijilv2zhuangbei</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dlsuijilv1zhuangbei</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>Name</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>sq隐秘石门</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>sucaidai;kapaibugeibao(wu);xiaoxingmofayaoji;jingyanzhishu;suijihuanshouka</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>15;20;20;20;25</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dlshimen</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dlzhuangbei2</t>
+  </si>
+  <si>
+    <t>dlzhuangbei3</t>
+  </si>
+  <si>
+    <t>dlzhuangbei4</t>
+  </si>
+  <si>
+    <t>dlzhuangbei5</t>
+  </si>
+  <si>
+    <t>dlzhuangbei1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1450,8 +1465,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:I40" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" tableBorderDxfId="6">
-  <autoFilter ref="A3:I40"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:I41" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" tableBorderDxfId="6">
+  <autoFilter ref="A3:I41"/>
   <sortState ref="A4:S80">
     <sortCondition ref="A3:A80"/>
   </sortState>
@@ -1791,13 +1806,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1875,7 +1890,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>97</v>
@@ -1907,7 +1922,7 @@
         <v>27</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D4" t="s">
         <v>60</v>
@@ -1930,7 +1945,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>61</v>
@@ -1950,7 +1965,7 @@
         <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>62</v>
@@ -1973,7 +1988,7 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D7" t="s">
         <v>63</v>
@@ -1993,7 +2008,7 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D8" t="s">
         <v>64</v>
@@ -2013,7 +2028,7 @@
         <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -2033,7 +2048,7 @@
         <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -2053,7 +2068,7 @@
         <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>99</v>
+        <v>137</v>
       </c>
       <c r="F11">
         <v>2</v>
@@ -2073,7 +2088,7 @@
         <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>100</v>
+        <v>138</v>
       </c>
       <c r="F12">
         <v>3</v>
@@ -2093,7 +2108,7 @@
         <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>101</v>
+        <v>139</v>
       </c>
       <c r="F13">
         <v>4</v>
@@ -2113,7 +2128,7 @@
         <v>28</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H14" t="s">
         <v>22</v>
@@ -2130,7 +2145,7 @@
         <v>29</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H15" t="s">
         <v>23</v>
@@ -2147,7 +2162,7 @@
         <v>30</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H16" t="s">
         <v>24</v>
@@ -2164,7 +2179,7 @@
         <v>31</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="H17" t="s">
         <v>25</v>
@@ -2181,7 +2196,7 @@
         <v>32</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D18" t="s">
         <v>65</v>
@@ -2201,7 +2216,7 @@
         <v>33</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D19" t="s">
         <v>66</v>
@@ -2221,7 +2236,7 @@
         <v>34</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D20" t="s">
         <v>67</v>
@@ -2241,7 +2256,7 @@
         <v>35</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D21" t="s">
         <v>68</v>
@@ -2261,7 +2276,7 @@
         <v>36</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D22" t="s">
         <v>69</v>
@@ -2281,7 +2296,7 @@
         <v>37</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D23" t="s">
         <v>70</v>
@@ -2301,7 +2316,7 @@
         <v>38</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>71</v>
@@ -2321,7 +2336,7 @@
         <v>39</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>72</v>
@@ -2341,7 +2356,7 @@
         <v>40</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>73</v>
@@ -2361,7 +2376,7 @@
         <v>41</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>74</v>
@@ -2381,7 +2396,7 @@
         <v>42</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>75</v>
@@ -2401,7 +2416,7 @@
         <v>43</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>76</v>
@@ -2421,7 +2436,7 @@
         <v>44</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D30" s="8" t="s">
         <v>77</v>
@@ -2441,7 +2456,7 @@
         <v>45</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D31" s="8" t="s">
         <v>78</v>
@@ -2461,7 +2476,7 @@
         <v>46</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D32" s="8" t="s">
         <v>79</v>
@@ -2481,7 +2496,7 @@
         <v>47</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D33" s="8" t="s">
         <v>80</v>
@@ -2501,7 +2516,7 @@
         <v>48</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D34" s="8" t="s">
         <v>81</v>
@@ -2521,7 +2536,7 @@
         <v>49</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D35" s="8" t="s">
         <v>82</v>
@@ -2541,7 +2556,7 @@
         <v>50</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D36" s="8" t="s">
         <v>83</v>
@@ -2561,7 +2576,7 @@
         <v>51</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D37" s="8" t="s">
         <v>84</v>
@@ -2581,7 +2596,7 @@
         <v>52</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D38" s="8" t="s">
         <v>85</v>
@@ -2601,7 +2616,7 @@
         <v>53</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D39" s="8" t="s">
         <v>86</v>
@@ -2621,7 +2636,7 @@
         <v>54</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D40" s="8" t="s">
         <v>87</v>
@@ -2631,6 +2646,26 @@
       </c>
       <c r="I40" s="3">
         <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A41">
+        <v>23000501</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="I41" s="3">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finish a new event waterbeast
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Drop.xlsx
+++ b/ConfigData/Xlsx/Drop.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Drop" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="149">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -513,13 +513,29 @@
   </si>
   <si>
     <t>15;15;40;30</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>sq传说水怪</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dlwaterbeast</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>sucaidai(shui);kapaibugeibao(shui);ziyuandai(yu);zhongxinghuoliyaoji;xiaoxingmofayaoji</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>15;10;25;15;35</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1481,21 +1497,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表2" displayName="表2" ref="A3:I42" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" tableBorderDxfId="6">
-  <autoFilter ref="A3:I42" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:I43" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" tableBorderDxfId="6">
+  <autoFilter ref="A3:I43"/>
   <sortState ref="A4:S80">
     <sortCondition ref="A3:A80"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Ename" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Items" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="ItemRate" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="EquipQualityMin"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="EquipQualityMax"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="RandomItemRate"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Count" dataDxfId="0"/>
+    <tableColumn id="1" name="Id" dataDxfId="5"/>
+    <tableColumn id="2" name="Name" dataDxfId="4"/>
+    <tableColumn id="7" name="Ename" dataDxfId="3"/>
+    <tableColumn id="12" name="Items" dataDxfId="2"/>
+    <tableColumn id="6" name="ItemRate" dataDxfId="1"/>
+    <tableColumn id="3" name="EquipQualityMin"/>
+    <tableColumn id="5" name="EquipQualityMax"/>
+    <tableColumn id="4" name="RandomItemRate"/>
+    <tableColumn id="13" name="Count" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1821,14 +1837,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G42" sqref="G42"/>
+      <selection pane="bottomRight" activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2704,6 +2720,26 @@
         <v>1</v>
       </c>
     </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A43">
+        <v>23000503</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="I43" s="3">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="H14:H17">

</xml_diff>

<commit_message>
a new quest of thief
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Drop.xlsx
+++ b/ConfigData/Xlsx/Drop.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="157">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -544,6 +544,22 @@
   </si>
   <si>
     <t>一个愿望</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>盗贼II</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dlthief</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>suijihuanshouka;suijihuanshouka;sucaidai(an);xiaoxinghuoliyaoji</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>15;15;30;40</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1294,16 +1310,6 @@
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="10">
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1516,6 +1522,16 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1530,21 +1546,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表2" displayName="表2" ref="A3:I44" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7">
-  <autoFilter ref="A3:I44" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表2" displayName="表2" ref="A3:I45" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" tableBorderDxfId="6">
+  <autoFilter ref="A3:I45" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <sortState ref="A4:S80">
     <sortCondition ref="A3:A80"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Ename" dataDxfId="4"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Items" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="ItemRate" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Ename" dataDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Items" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="ItemRate" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="EquipQualityMin"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="EquipQualityMax"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="RandomItemRate"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Count" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Count" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1871,13 +1887,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B44" sqref="B44"/>
+      <selection pane="bottomRight" activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2793,10 +2809,30 @@
         <v>1</v>
       </c>
     </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A45">
+        <v>23000505</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="I45" s="3">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="H14:H17">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="9" priority="1">
       <formula>LEN(TRIM(H14))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add new quest for cards
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Drop.xlsx
+++ b/ConfigData/Xlsx/Drop.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Drop" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -472,14 +472,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>sucaidai;kapaibugeibao(wu);xiaoxingmofayaoji;jingyanzhishu;suijihuanshouka</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>15;20;20;20;25</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>dlshimen</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -508,14 +500,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>ziyuandai(lan);kapaibugeibao(shui);zycao2;zycao4</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>15;15;40;30</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>sq传说水怪</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -524,49 +508,66 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>sucaidai(shui);kapaibugeibao(shui);ziyuandai(yu);zhongxinghuoliyaoji;xiaoxingmofayaoji</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>15;10;25;15;35</t>
+    <t>25;25;25;25</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dlwishwell</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>一个愿望</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>盗贼II</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dlthief</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>suijihuanshouka;suijihuanshouka;sucaidai(an);xiaoxinghuoliyaoji</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>15;15;30;40</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>sucaidai;xiaoxingmofayaoji;jingyanzhishu;suijihuanshouka</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>15;20;20;25</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ziyuandai(lan);zycao2;zycao4</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>sucaidai(shui);ziyuandai(yu);zhongxinghuoliyaoji;xiaoxingmofayaoji</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>15;25;15;35</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>15;40;30</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>shuiyinbugeiche2;hongbaoshibugeiche2;liuhuangbugeiche2;shuijingbugeiche2</t>
-  </si>
-  <si>
-    <t>25;25;25;25</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dlwishwell</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>一个愿望</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>盗贼II</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dlthief</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>suijihuanshouka;suijihuanshouka;sucaidai(an);xiaoxinghuoliyaoji</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>15;15;30;40</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1546,21 +1547,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表2" displayName="表2" ref="A3:I45" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" tableBorderDxfId="6">
-  <autoFilter ref="A3:I45" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:I45" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" tableBorderDxfId="6">
+  <autoFilter ref="A3:I45"/>
   <sortState ref="A4:S80">
     <sortCondition ref="A3:A80"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Ename" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Items" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="ItemRate" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="EquipQualityMin"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="EquipQualityMax"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="RandomItemRate"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Count" dataDxfId="0"/>
+    <tableColumn id="1" name="Id" dataDxfId="5"/>
+    <tableColumn id="2" name="Name" dataDxfId="4"/>
+    <tableColumn id="7" name="Ename" dataDxfId="3"/>
+    <tableColumn id="12" name="Items" dataDxfId="2"/>
+    <tableColumn id="6" name="ItemRate" dataDxfId="1"/>
+    <tableColumn id="3" name="EquipQualityMin"/>
+    <tableColumn id="5" name="EquipQualityMax"/>
+    <tableColumn id="4" name="RandomItemRate"/>
+    <tableColumn id="13" name="Count" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1886,14 +1887,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C45" sqref="C45"/>
+      <selection pane="bottomRight" activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2109,7 +2110,7 @@
         <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -2129,7 +2130,7 @@
         <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -2149,7 +2150,7 @@
         <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F11">
         <v>2</v>
@@ -2169,7 +2170,7 @@
         <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F12">
         <v>3</v>
@@ -2189,7 +2190,7 @@
         <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F13">
         <v>4</v>
@@ -2737,13 +2738,13 @@
         <v>132</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>133</v>
+        <v>150</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>134</v>
+        <v>151</v>
       </c>
       <c r="I41" s="3">
         <v>2</v>
@@ -2754,16 +2755,16 @@
         <v>23000502</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
       <c r="I42" s="3">
         <v>1</v>
@@ -2774,16 +2775,16 @@
         <v>23000503</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="I43" s="3">
         <v>3</v>
@@ -2794,16 +2795,16 @@
         <v>23000504</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="I44" s="3">
         <v>1</v>
@@ -2814,16 +2815,16 @@
         <v>23000505</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="I45" s="3">
         <v>2</v>

</xml_diff>

<commit_message>
optimise the equip compose system
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Drop.xlsx
+++ b/ConfigData/Xlsx/Drop.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="151">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -70,10 +70,6 @@
     <t>枯木</t>
   </si>
   <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>随机Lv1装备</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -214,26 +210,6 @@
   </si>
   <si>
     <t>资源袋(石像)</t>
-  </si>
-  <si>
-    <t>装备品质最低</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>装备品质最高</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>EquipQualityMin</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>EquipQualityMax</t>
-    <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>zycao1;zycao2;zycao3;zycao4;zycao5;zycao6;zycao7;zycao8</t>
@@ -756,7 +732,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -950,14 +926,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
-        <bgColor theme="4"/>
       </patternFill>
     </fill>
   </fills>
@@ -1225,7 +1195,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1253,17 +1223,11 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="255" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="255" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1311,6 +1275,16 @@
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="10">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1523,16 +1497,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1547,21 +1511,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:I45" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" tableBorderDxfId="6">
-  <autoFilter ref="A3:I45"/>
-  <sortState ref="A4:S80">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:G45" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7">
+  <autoFilter ref="A3:G45"/>
+  <sortState ref="A4:Q80">
     <sortCondition ref="A3:A80"/>
   </sortState>
-  <tableColumns count="9">
-    <tableColumn id="1" name="Id" dataDxfId="5"/>
-    <tableColumn id="2" name="Name" dataDxfId="4"/>
-    <tableColumn id="7" name="Ename" dataDxfId="3"/>
-    <tableColumn id="12" name="Items" dataDxfId="2"/>
-    <tableColumn id="6" name="ItemRate" dataDxfId="1"/>
-    <tableColumn id="3" name="EquipQualityMin"/>
-    <tableColumn id="5" name="EquipQualityMax"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Id" dataDxfId="6"/>
+    <tableColumn id="2" name="Name" dataDxfId="5"/>
+    <tableColumn id="7" name="Ename" dataDxfId="4"/>
+    <tableColumn id="12" name="Items" dataDxfId="3"/>
+    <tableColumn id="6" name="ItemRate" dataDxfId="2"/>
     <tableColumn id="4" name="RandomItemRate"/>
-    <tableColumn id="13" name="Count" dataDxfId="0"/>
+    <tableColumn id="13" name="Count" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1888,13 +1850,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D45" sqref="D45"/>
+      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1904,41 +1866,34 @@
     <col min="3" max="3" width="9.875" customWidth="1"/>
     <col min="4" max="4" width="48.75" customWidth="1"/>
     <col min="5" max="5" width="21.875" customWidth="1"/>
-    <col min="6" max="7" width="4.25" customWidth="1"/>
-    <col min="8" max="8" width="15.875" customWidth="1"/>
-    <col min="9" max="9" width="4.25" customWidth="1"/>
+    <col min="6" max="6" width="15.875" customWidth="1"/>
+    <col min="7" max="7" width="4.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1949,77 +1904,63 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>23000001</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="D4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E4" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G4" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>23000002</v>
       </c>
@@ -2027,42 +1968,40 @@
         <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="I5" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+        <v>82</v>
+      </c>
+      <c r="G5" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>23000003</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G6" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>23000004</v>
       </c>
@@ -2070,19 +2009,19 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D7" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E7" t="s">
-        <v>89</v>
-      </c>
-      <c r="I7" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+        <v>83</v>
+      </c>
+      <c r="G7" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>23000005</v>
       </c>
@@ -2090,751 +2029,736 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D8" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E8" t="s">
-        <v>90</v>
-      </c>
-      <c r="I8" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+        <v>84</v>
+      </c>
+      <c r="G8" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>23000101</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>138</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>3</v>
-      </c>
-      <c r="I9" s="3">
+        <v>132</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>23000102</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>134</v>
-      </c>
-      <c r="F10">
+        <v>128</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="G10" s="3">
         <v>1</v>
       </c>
-      <c r="G10">
-        <v>3</v>
-      </c>
-      <c r="I10" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>23000103</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>135</v>
-      </c>
-      <c r="F11">
-        <v>2</v>
-      </c>
-      <c r="G11">
-        <v>3</v>
-      </c>
-      <c r="I11" s="3">
+        <v>129</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>23000104</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>136</v>
-      </c>
-      <c r="F12">
-        <v>3</v>
-      </c>
-      <c r="G12">
-        <v>3</v>
-      </c>
-      <c r="I12" s="3">
+        <v>130</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>23000105</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>137</v>
-      </c>
-      <c r="F13">
-        <v>4</v>
-      </c>
-      <c r="G13">
-        <v>4</v>
-      </c>
-      <c r="I13" s="3">
+        <v>131</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="G13" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>23000201</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="H14" t="s">
-        <v>22</v>
-      </c>
-      <c r="I14" s="3">
+        <v>121</v>
+      </c>
+      <c r="F14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>23000202</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="H15" t="s">
-        <v>23</v>
-      </c>
-      <c r="I15" s="3">
+        <v>122</v>
+      </c>
+      <c r="F15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>23000203</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="H16" t="s">
-        <v>24</v>
-      </c>
-      <c r="I16" s="3">
+        <v>123</v>
+      </c>
+      <c r="F16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>23000204</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="H17" t="s">
-        <v>25</v>
-      </c>
-      <c r="I17" s="3">
+        <v>124</v>
+      </c>
+      <c r="F17" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>23000301</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D18" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E18" t="s">
-        <v>91</v>
-      </c>
-      <c r="I18" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+        <v>85</v>
+      </c>
+      <c r="G18" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>23000302</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D19" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E19" t="s">
-        <v>91</v>
-      </c>
-      <c r="I19" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+        <v>85</v>
+      </c>
+      <c r="G19" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>23000303</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D20" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E20" t="s">
-        <v>91</v>
-      </c>
-      <c r="I20" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+        <v>85</v>
+      </c>
+      <c r="G20" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>23000304</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D21" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E21" t="s">
-        <v>91</v>
-      </c>
-      <c r="I21" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+        <v>85</v>
+      </c>
+      <c r="G21" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>23000305</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D22" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E22" t="s">
-        <v>91</v>
-      </c>
-      <c r="I22" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
+        <v>85</v>
+      </c>
+      <c r="G22" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>23000306</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D23" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E23" t="s">
-        <v>91</v>
-      </c>
-      <c r="I23" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
+        <v>85</v>
+      </c>
+      <c r="G23" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>23000307</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="I24" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
+        <v>85</v>
+      </c>
+      <c r="G24" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>23000401</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="I25" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+        <v>86</v>
+      </c>
+      <c r="G25" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>23000402</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="I26" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
+        <v>86</v>
+      </c>
+      <c r="G26" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>23000403</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="I27" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
+        <v>86</v>
+      </c>
+      <c r="G27" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>23000404</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="I28" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
+        <v>86</v>
+      </c>
+      <c r="G28" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>23000405</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="I29" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
+        <v>86</v>
+      </c>
+      <c r="G29" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>23000406</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="I30" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
+        <v>86</v>
+      </c>
+      <c r="G30" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>23000407</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="I31" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
+        <v>86</v>
+      </c>
+      <c r="G31" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>23000408</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="I32" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
+        <v>86</v>
+      </c>
+      <c r="G32" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>23000409</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="I33" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
+        <v>86</v>
+      </c>
+      <c r="G33" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>23000410</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="I34" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
+        <v>86</v>
+      </c>
+      <c r="G34" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>23000411</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="I35" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
+        <v>86</v>
+      </c>
+      <c r="G35" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>23000412</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="I36" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
+        <v>86</v>
+      </c>
+      <c r="G36" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>23000413</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="I37" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
+        <v>86</v>
+      </c>
+      <c r="G37" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>23000414</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="I38" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
+        <v>86</v>
+      </c>
+      <c r="G38" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>23000415</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D39" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E39" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E39" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="I39" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G39" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>23000416</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="I40" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
+        <v>86</v>
+      </c>
+      <c r="G40" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>23000501</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="I41" s="3">
+        <v>145</v>
+      </c>
+      <c r="G41" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A42">
         <v>23000502</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="I42" s="3">
+        <v>149</v>
+      </c>
+      <c r="G42" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A43">
         <v>23000503</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="I43" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.15">
+        <v>148</v>
+      </c>
+      <c r="G43" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A44">
         <v>23000504</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="I44" s="3">
+        <v>137</v>
+      </c>
+      <c r="G44" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>23000505</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="I45" s="3">
+        <v>143</v>
+      </c>
+      <c r="G45" s="3">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="H14:H17">
-    <cfRule type="containsBlanks" dxfId="9" priority="1">
-      <formula>LEN(TRIM(H14))=0</formula>
+  <conditionalFormatting sqref="F14:F17">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(F14))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
support drop equips for quests
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Drop.xlsx
+++ b/ConfigData/Xlsx/Drop.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="154">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -93,9 +93,6 @@
     <t>随机素材概率</t>
   </si>
   <si>
-    <t>RandomItemRate</t>
-  </si>
-  <si>
     <t>35;27;22;15;1;0;0</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -537,6 +534,22 @@
   </si>
   <si>
     <t>shuiyinbugeiche2;hongbaoshibugeiche2;liuhuangbugeiche2;shuijingbugeiche2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>MaterialRate</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>是否掉落随机装备</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>DropEquip</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>double</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -926,7 +939,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1195,7 +1208,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1226,7 +1239,16 @@
     <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="255" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1274,17 +1296,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <font>
         <b val="0"/>
@@ -1511,19 +1523,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:G45" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7">
-  <autoFilter ref="A3:G45"/>
-  <sortState ref="A4:Q80">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:H45" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" tableBorderDxfId="6">
+  <autoFilter ref="A3:H45"/>
+  <sortState ref="A4:R80">
     <sortCondition ref="A3:A80"/>
   </sortState>
-  <tableColumns count="7">
-    <tableColumn id="1" name="Id" dataDxfId="6"/>
-    <tableColumn id="2" name="Name" dataDxfId="5"/>
-    <tableColumn id="7" name="Ename" dataDxfId="4"/>
-    <tableColumn id="12" name="Items" dataDxfId="3"/>
-    <tableColumn id="6" name="ItemRate" dataDxfId="2"/>
-    <tableColumn id="4" name="RandomItemRate"/>
-    <tableColumn id="13" name="Count" dataDxfId="1"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="Id" dataDxfId="5"/>
+    <tableColumn id="2" name="Name" dataDxfId="4"/>
+    <tableColumn id="7" name="Ename" dataDxfId="3"/>
+    <tableColumn id="12" name="Items" dataDxfId="2"/>
+    <tableColumn id="6" name="ItemRate" dataDxfId="1"/>
+    <tableColumn id="4" name="MaterialRate"/>
+    <tableColumn id="3" name="DropEquip"/>
+    <tableColumn id="13" name="Count" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1850,13 +1863,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomRight" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1867,10 +1880,11 @@
     <col min="4" max="4" width="48.75" customWidth="1"/>
     <col min="5" max="5" width="21.875" customWidth="1"/>
     <col min="6" max="6" width="15.875" customWidth="1"/>
-    <col min="7" max="7" width="4.25" customWidth="1"/>
+    <col min="7" max="7" width="6.375" customWidth="1"/>
+    <col min="8" max="8" width="4.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="9" t="s">
         <v>2</v>
       </c>
@@ -1878,22 +1892,25 @@
         <v>3</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>19</v>
       </c>
       <c r="G1" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1904,144 +1921,152 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>88</v>
-      </c>
       <c r="F2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>20</v>
+        <v>150</v>
       </c>
       <c r="G3" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>23000001</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="D4" t="s">
-        <v>54</v>
+      <c r="B4" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>53</v>
       </c>
       <c r="E4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F4" s="3"/>
-      <c r="G4" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G4" s="3"/>
+      <c r="H4" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>23000002</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>55</v>
+      <c r="C5" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>54</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="G5" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+      <c r="H5" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>23000003</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s">
-        <v>118</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>56</v>
+      <c r="C6" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>55</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F6" s="3"/>
-      <c r="G6" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G6" s="3"/>
+      <c r="H6" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>23000004</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C7" t="s">
-        <v>119</v>
-      </c>
-      <c r="D7" t="s">
-        <v>57</v>
+      <c r="C7" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>56</v>
       </c>
       <c r="E7" t="s">
-        <v>83</v>
-      </c>
-      <c r="G7" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+        <v>82</v>
+      </c>
+      <c r="H7" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>23000005</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C8" t="s">
-        <v>120</v>
-      </c>
-      <c r="D8" t="s">
-        <v>58</v>
+      <c r="C8" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="E8" t="s">
-        <v>84</v>
-      </c>
-      <c r="G8" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+        <v>83</v>
+      </c>
+      <c r="H8" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>23000101</v>
       </c>
@@ -2049,16 +2074,16 @@
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>132</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="G9" s="3">
+        <v>131</v>
+      </c>
+      <c r="G9" s="13">
+        <v>0.4</v>
+      </c>
+      <c r="H9" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>23000102</v>
       </c>
@@ -2066,16 +2091,16 @@
         <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>128</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="G10" s="3">
+        <v>127</v>
+      </c>
+      <c r="G10" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="H10" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>23000103</v>
       </c>
@@ -2083,16 +2108,16 @@
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>129</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="G11" s="3">
+        <v>128</v>
+      </c>
+      <c r="G11" s="13">
+        <v>0.6</v>
+      </c>
+      <c r="H11" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>23000104</v>
       </c>
@@ -2100,16 +2125,16 @@
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>130</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="G12" s="3">
+        <v>129</v>
+      </c>
+      <c r="G12" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="H12" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>23000105</v>
       </c>
@@ -2117,650 +2142,645 @@
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>131</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="G13" s="3">
+        <v>130</v>
+      </c>
+      <c r="G13" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H13" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>23000201</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F14" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14" s="3">
+        <v>20</v>
+      </c>
+      <c r="H14" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>23000202</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F15" t="s">
-        <v>22</v>
-      </c>
-      <c r="G15" s="3">
+        <v>21</v>
+      </c>
+      <c r="H15" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>23000203</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F16" t="s">
-        <v>23</v>
-      </c>
-      <c r="G16" s="3">
+        <v>22</v>
+      </c>
+      <c r="H16" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>23000204</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F17" t="s">
-        <v>24</v>
-      </c>
-      <c r="G17" s="3">
+        <v>23</v>
+      </c>
+      <c r="H17" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>23000301</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E18" t="s">
-        <v>85</v>
-      </c>
-      <c r="G18" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+        <v>84</v>
+      </c>
+      <c r="H18" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>23000302</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E19" t="s">
-        <v>85</v>
-      </c>
-      <c r="G19" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
+        <v>84</v>
+      </c>
+      <c r="H19" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>23000303</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E20" t="s">
-        <v>85</v>
-      </c>
-      <c r="G20" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
+        <v>84</v>
+      </c>
+      <c r="H20" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>23000304</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E21" t="s">
-        <v>85</v>
-      </c>
-      <c r="G21" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
+        <v>84</v>
+      </c>
+      <c r="H21" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>23000305</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E22" t="s">
-        <v>85</v>
-      </c>
-      <c r="G22" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
+        <v>84</v>
+      </c>
+      <c r="H22" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>23000306</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E23" t="s">
-        <v>85</v>
-      </c>
-      <c r="G23" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
+        <v>84</v>
+      </c>
+      <c r="H23" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>23000307</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="G24" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
+        <v>84</v>
+      </c>
+      <c r="H24" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>23000401</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G25" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
+        <v>85</v>
+      </c>
+      <c r="H25" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>23000402</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G26" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
+        <v>85</v>
+      </c>
+      <c r="H26" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>23000403</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G27" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
+        <v>85</v>
+      </c>
+      <c r="H27" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>23000404</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G28" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
+        <v>85</v>
+      </c>
+      <c r="H28" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>23000405</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G29" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
+        <v>85</v>
+      </c>
+      <c r="H29" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>23000406</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G30" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
+        <v>85</v>
+      </c>
+      <c r="H30" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>23000407</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G31" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
+        <v>85</v>
+      </c>
+      <c r="H31" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>23000408</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G32" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
+        <v>85</v>
+      </c>
+      <c r="H32" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>23000409</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G33" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
+        <v>85</v>
+      </c>
+      <c r="H33" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>23000410</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G34" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
+        <v>85</v>
+      </c>
+      <c r="H34" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>23000411</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G35" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
+        <v>85</v>
+      </c>
+      <c r="H35" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>23000412</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G36" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
+        <v>85</v>
+      </c>
+      <c r="H36" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>23000413</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G37" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
+        <v>85</v>
+      </c>
+      <c r="H37" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>23000414</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G38" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
+        <v>85</v>
+      </c>
+      <c r="H38" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>23000415</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G39" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
+        <v>85</v>
+      </c>
+      <c r="H39" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>23000416</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G40" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
+        <v>85</v>
+      </c>
+      <c r="H40" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>23000501</v>
       </c>
       <c r="B41" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>127</v>
-      </c>
       <c r="D41" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="E41" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="E41" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="G41" s="3">
+      <c r="H41" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A42">
         <v>23000502</v>
       </c>
       <c r="B42" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C42" s="3" t="s">
-        <v>134</v>
-      </c>
       <c r="D42" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="G42" s="3">
+        <v>148</v>
+      </c>
+      <c r="H42" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A43">
         <v>23000503</v>
       </c>
       <c r="B43" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C43" s="3" t="s">
-        <v>136</v>
-      </c>
       <c r="D43" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="E43" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="E43" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="G43" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H43" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A44">
         <v>23000504</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="G44" s="3">
+        <v>136</v>
+      </c>
+      <c r="H44" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>23000505</v>
       </c>
       <c r="B45" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C45" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="D45" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="D45" s="6" t="s">
+      <c r="E45" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="E45" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="G45" s="3">
+      <c r="H45" s="3">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="F14:F17">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(F14))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
add some new veges
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Drop.xlsx
+++ b/ConfigData/Xlsx/Drop.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{A5A61867-765E-40FA-9182-DBE17B113397}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Drop" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="140">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -60,16 +61,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>水池</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>蘑菇</t>
-  </si>
-  <si>
-    <t>枯木</t>
-  </si>
-  <si>
     <t>随机Lv1装备</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -86,10 +77,6 @@
     <t>随机Lv5装备</t>
   </si>
   <si>
-    <t>矿洞</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>随机素材概率</t>
   </si>
   <si>
@@ -113,10 +100,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>草丛</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>素材袋</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -209,21 +192,6 @@
     <t>资源袋(石像)</t>
   </si>
   <si>
-    <t>zycao1;zycao2;zycao3;zycao4;zycao5;zycao6;zycao7;zycao8</t>
-  </si>
-  <si>
-    <t>zyyu1;zyyu2;zyyu3;zyyu4;zyyu5;zyyu6;zyyu7;zyyu8</t>
-  </si>
-  <si>
-    <t>zyshi1;zyshi2;zyshi3;zyshi4;zyshi5;zyshi6;zyshi7;zyshi8</t>
-  </si>
-  <si>
-    <t>zygu1;zygu2;zygu3</t>
-  </si>
-  <si>
-    <t>zymu1;zymu2;zymu3;zymu4</t>
-  </si>
-  <si>
     <t>scwu1;scwu2;scwu3;scwu4</t>
   </si>
   <si>
@@ -293,15 +261,6 @@
     <t>sctuteng1;sctuteng2;sctuteng3;sctuteng4</t>
   </si>
   <si>
-    <t>32;28;15;12;6;4;2;1</t>
-  </si>
-  <si>
-    <t>30;15;7</t>
-  </si>
-  <si>
-    <t>30;15;4;3</t>
-  </si>
-  <si>
     <t>52;28;15;5</t>
   </si>
   <si>
@@ -401,26 +360,6 @@
     <t>dlziyuandai(shixiang)</t>
   </si>
   <si>
-    <t>dlcao</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dlyu</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dlshi</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dlgu</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dlmu</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>dlsucaidai</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -550,13 +489,28 @@
   </si>
   <si>
     <t>double</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dlsigua</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>丝瓜</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>zzwandou;zzyumi;zzpingguo;zzlanmei;zznangua;zzxihongshi;zzqiezi;zzluobo;zztudou;zzlajiao;zzyangcong</t>
+  </si>
+  <si>
+    <t>9;9;9;9;9;9;9;9;9;9;9</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -745,7 +699,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -935,12 +889,6 @@
       <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor theme="4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1239,16 +1187,16 @@
     <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="255" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1523,20 +1471,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:H45" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" tableBorderDxfId="6">
-  <autoFilter ref="A3:H45"/>
-  <sortState ref="A4:R80">
-    <sortCondition ref="A3:A80"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表2" displayName="表2" ref="A3:H41" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" tableBorderDxfId="6">
+  <autoFilter ref="A3:H41" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState ref="A4:R76">
+    <sortCondition ref="A3:A76"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" name="Id" dataDxfId="5"/>
-    <tableColumn id="2" name="Name" dataDxfId="4"/>
-    <tableColumn id="7" name="Ename" dataDxfId="3"/>
-    <tableColumn id="12" name="Items" dataDxfId="2"/>
-    <tableColumn id="6" name="ItemRate" dataDxfId="1"/>
-    <tableColumn id="4" name="MaterialRate"/>
-    <tableColumn id="3" name="DropEquip"/>
-    <tableColumn id="13" name="Count" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Ename" dataDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Items" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="ItemRate" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="MaterialRate"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="DropEquip"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Count" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1862,14 +1810,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1892,19 +1840,19 @@
         <v>3</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>7</v>
@@ -1921,16 +1869,16 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>8</v>
@@ -1941,22 +1889,22 @@
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>9</v>
@@ -1966,17 +1914,17 @@
       <c r="A4">
         <v>23000001</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>53</v>
+      <c r="B4" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>138</v>
       </c>
       <c r="E4" t="s">
-        <v>81</v>
+        <v>139</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -1986,98 +1934,84 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5">
-        <v>23000002</v>
-      </c>
-      <c r="B5" s="10" t="s">
+        <v>23000101</v>
+      </c>
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>81</v>
+      <c r="C5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G5" s="10">
+        <v>0.4</v>
       </c>
       <c r="H5" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6">
-        <v>23000003</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+        <v>23000102</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>109</v>
+      </c>
+      <c r="G6" s="10">
+        <v>0.5</v>
+      </c>
       <c r="H6" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7">
-        <v>23000004</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="E7" t="s">
-        <v>82</v>
+        <v>23000103</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>110</v>
+      </c>
+      <c r="G7" s="10">
+        <v>0.6</v>
       </c>
       <c r="H7" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A8">
-        <v>23000005</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="E8" t="s">
-        <v>83</v>
+        <v>23000104</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>111</v>
+      </c>
+      <c r="G8" s="10">
+        <v>0.8</v>
       </c>
       <c r="H8" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A9">
-        <v>23000101</v>
+        <v>23000105</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>131</v>
-      </c>
-      <c r="G9" s="13">
-        <v>0.4</v>
+        <v>112</v>
+      </c>
+      <c r="G9" s="10">
+        <v>1</v>
       </c>
       <c r="H9" s="3">
         <v>1</v>
@@ -2085,155 +2019,167 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10">
-        <v>23000102</v>
-      </c>
-      <c r="B10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>127</v>
-      </c>
-      <c r="G10" s="13">
-        <v>0.5</v>
+        <v>23000201</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F10" t="s">
+        <v>16</v>
       </c>
       <c r="H10" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A11">
-        <v>23000103</v>
-      </c>
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" t="s">
-        <v>128</v>
-      </c>
-      <c r="G11" s="13">
-        <v>0.6</v>
+        <v>23000202</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="F11" t="s">
+        <v>17</v>
       </c>
       <c r="H11" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A12">
-        <v>23000104</v>
-      </c>
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" t="s">
-        <v>129</v>
-      </c>
-      <c r="G12" s="13">
-        <v>0.8</v>
+        <v>23000203</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="F12" t="s">
+        <v>18</v>
       </c>
       <c r="H12" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A13">
-        <v>23000105</v>
-      </c>
-      <c r="B13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" t="s">
-        <v>130</v>
-      </c>
-      <c r="G13" s="13">
-        <v>1</v>
+        <v>23000204</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F13" t="s">
+        <v>19</v>
       </c>
       <c r="H13" s="3">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A14">
-        <v>23000201</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="F14" t="s">
-        <v>20</v>
+        <v>23000301</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" t="s">
+        <v>71</v>
       </c>
       <c r="H14" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A15">
-        <v>23000202</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="F15" t="s">
-        <v>21</v>
+        <v>23000302</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" t="s">
+        <v>71</v>
       </c>
       <c r="H15" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A16">
-        <v>23000203</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="F16" t="s">
-        <v>22</v>
+        <v>23000303</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" t="s">
+        <v>71</v>
       </c>
       <c r="H16" s="3">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A17">
-        <v>23000204</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F17" t="s">
-        <v>23</v>
+        <v>23000304</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" t="s">
+        <v>71</v>
       </c>
       <c r="H17" s="3">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A18">
-        <v>23000301</v>
+        <v>23000305</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="D18" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E18" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="H18" s="3">
         <v>3</v>
@@ -2241,19 +2187,19 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A19">
-        <v>23000302</v>
+        <v>23000306</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="D19" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E19" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="H19" s="3">
         <v>3</v>
@@ -2261,19 +2207,19 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A20">
-        <v>23000303</v>
+        <v>23000307</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="D20" t="s">
-        <v>60</v>
-      </c>
-      <c r="E20" t="s">
-        <v>84</v>
+        <v>31</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>71</v>
       </c>
       <c r="H20" s="3">
         <v>3</v>
@@ -2281,19 +2227,19 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A21">
-        <v>23000304</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="D21" t="s">
-        <v>61</v>
-      </c>
-      <c r="E21" t="s">
-        <v>84</v>
+        <v>23000401</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>72</v>
       </c>
       <c r="H21" s="3">
         <v>3</v>
@@ -2301,19 +2247,19 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A22">
-        <v>23000305</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="D22" t="s">
-        <v>62</v>
-      </c>
-      <c r="E22" t="s">
-        <v>84</v>
+        <v>23000402</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>72</v>
       </c>
       <c r="H22" s="3">
         <v>3</v>
@@ -2321,19 +2267,19 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A23">
-        <v>23000306</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D23" t="s">
-        <v>63</v>
-      </c>
-      <c r="E23" t="s">
-        <v>84</v>
+        <v>23000403</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>72</v>
       </c>
       <c r="H23" s="3">
         <v>3</v>
@@ -2341,19 +2287,19 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A24">
-        <v>23000307</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>98</v>
+        <v>23000404</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="H24" s="3">
         <v>3</v>
@@ -2361,19 +2307,19 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A25">
-        <v>23000401</v>
+        <v>23000405</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="H25" s="3">
         <v>3</v>
@@ -2381,19 +2327,19 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A26">
-        <v>23000402</v>
+        <v>23000406</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="H26" s="3">
         <v>3</v>
@@ -2401,19 +2347,19 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A27">
-        <v>23000403</v>
+        <v>23000407</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="H27" s="3">
         <v>3</v>
@@ -2421,19 +2367,19 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A28">
-        <v>23000404</v>
+        <v>23000408</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="H28" s="3">
         <v>3</v>
@@ -2441,19 +2387,19 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A29">
-        <v>23000405</v>
+        <v>23000409</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="H29" s="3">
         <v>3</v>
@@ -2461,19 +2407,19 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A30">
-        <v>23000406</v>
+        <v>23000410</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="H30" s="3">
         <v>3</v>
@@ -2481,19 +2427,19 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A31">
-        <v>23000407</v>
+        <v>23000411</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="H31" s="3">
         <v>3</v>
@@ -2501,19 +2447,19 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A32">
-        <v>23000408</v>
+        <v>23000412</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D32" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E32" s="8" t="s">
         <v>72</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="H32" s="3">
         <v>3</v>
@@ -2521,19 +2467,19 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A33">
-        <v>23000409</v>
+        <v>23000413</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="H33" s="3">
         <v>3</v>
@@ -2541,19 +2487,19 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A34">
-        <v>23000410</v>
+        <v>23000414</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="H34" s="3">
         <v>3</v>
@@ -2561,19 +2507,19 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A35">
-        <v>23000411</v>
+        <v>23000415</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="H35" s="3">
         <v>3</v>
@@ -2581,19 +2527,19 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A36">
-        <v>23000412</v>
+        <v>23000416</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="H36" s="3">
         <v>3</v>
@@ -2601,59 +2547,59 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A37">
-        <v>23000413</v>
+        <v>23000501</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>49</v>
+        <v>107</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>77</v>
+        <v>125</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>85</v>
+        <v>126</v>
       </c>
       <c r="H37" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A38">
-        <v>23000414</v>
+        <v>23000502</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>50</v>
+        <v>114</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>78</v>
+        <v>127</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>85</v>
+        <v>130</v>
       </c>
       <c r="H38" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A39">
-        <v>23000415</v>
+        <v>23000503</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>51</v>
+        <v>116</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>79</v>
+        <v>128</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>85</v>
+        <v>129</v>
       </c>
       <c r="H39" s="3">
         <v>3</v>
@@ -2661,121 +2607,41 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A40">
-        <v>23000416</v>
+        <v>23000504</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>52</v>
+        <v>120</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>80</v>
+        <v>131</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>85</v>
+        <v>118</v>
       </c>
       <c r="H40" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A41">
-        <v>23000501</v>
+        <v>23000505</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
       <c r="H41" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A42">
-        <v>23000502</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="E42" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="H42" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A43">
-        <v>23000503</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="E43" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="H43" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A44">
-        <v>23000504</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="H44" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A45">
-        <v>23000505</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="E45" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="H45" s="3">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
the building of wealth bay
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Drop.xlsx
+++ b/ConfigData/Xlsx/Drop.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{A5A61867-765E-40FA-9182-DBE17B113397}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Drop" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="142">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -504,14 +503,22 @@
   </si>
   <si>
     <t>9;9;9;9;9;9;9;9;9;9;9</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dlhaidaowan</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>海盗湾</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -698,6 +705,13 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -1156,7 +1170,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1197,6 +1211,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1459,6 +1479,74 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1471,20 +1559,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表2" displayName="表2" ref="A3:H41" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" tableBorderDxfId="6">
-  <autoFilter ref="A3:H41" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <sortState ref="A4:R76">
-    <sortCondition ref="A3:A76"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:H42" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" tableBorderDxfId="6">
+  <autoFilter ref="A3:H42"/>
+  <sortState ref="A4:H42">
+    <sortCondition ref="A3:A42"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Ename" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Items" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="ItemRate" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="MaterialRate"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="DropEquip"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Count" dataDxfId="0"/>
+    <tableColumn id="1" name="Id" dataDxfId="5"/>
+    <tableColumn id="2" name="Name" dataDxfId="4"/>
+    <tableColumn id="7" name="Ename" dataDxfId="3"/>
+    <tableColumn id="12" name="Items" dataDxfId="2"/>
+    <tableColumn id="6" name="ItemRate" dataDxfId="1"/>
+    <tableColumn id="4" name="MaterialRate"/>
+    <tableColumn id="3" name="DropEquip"/>
+    <tableColumn id="13" name="Count" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1498,7 +1586,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C7EDCC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1810,14 +1898,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomRight" activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1936,12 +2024,13 @@
       <c r="A5">
         <v>23000101</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="14" t="s">
         <v>113</v>
       </c>
+      <c r="D5" s="14"/>
       <c r="G5" s="10">
         <v>0.4</v>
       </c>
@@ -2021,7 +2110,7 @@
       <c r="A10">
         <v>23000201</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="7" t="s">
@@ -2212,10 +2301,10 @@
       <c r="B20" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="8" t="s">
         <v>54</v>
       </c>
       <c r="E20" s="8" t="s">
@@ -2643,6 +2732,28 @@
       </c>
       <c r="H41" s="3">
         <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A42">
+        <v>23010001</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="E42" t="s">
+        <v>139</v>
+      </c>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="15">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>